<commit_message>
more data entry, still not finished yet
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95238220-1329-4EC6-B800-71781052FC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49764788-8856-4E82-BC00-BFB1C0FB631A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>Chinese_Name</t>
   </si>
@@ -44,18 +44,6 @@
     <t>English_Name</t>
   </si>
   <si>
-    <t>Vocal_Rating</t>
-  </si>
-  <si>
-    <t>Dance_Rating</t>
-  </si>
-  <si>
-    <t>Physical_Rating</t>
-  </si>
-  <si>
-    <t>Overall_Rating</t>
-  </si>
-  <si>
     <t>Basic_Strength_Ranking</t>
   </si>
   <si>
@@ -234,6 +222,126 @@
   </si>
   <si>
     <t>Left the show due to health issues</t>
+  </si>
+  <si>
+    <t>Park Sun</t>
+  </si>
+  <si>
+    <t>Lee Yoo Jeong</t>
+  </si>
+  <si>
+    <t>Kim Na Yeon</t>
+  </si>
+  <si>
+    <t>Roh Ji Sun</t>
+  </si>
+  <si>
+    <t>Park Ji Won</t>
+  </si>
+  <si>
+    <t>Cho Yu Bin</t>
+  </si>
+  <si>
+    <t>Lee Sae Rom</t>
+  </si>
+  <si>
+    <t>Som Hye In</t>
+  </si>
+  <si>
+    <t>Yoo Ji Na</t>
+  </si>
+  <si>
+    <t>Lee Si An</t>
+  </si>
+  <si>
+    <t>Jung So Mi</t>
+  </si>
+  <si>
+    <t>Lee Da Hee</t>
+  </si>
+  <si>
+    <t>Sky / Bin Ha Neul</t>
+  </si>
+  <si>
+    <t>Lee Seo Yeon</t>
+  </si>
+  <si>
+    <t>Yang Yeon Ji</t>
+  </si>
+  <si>
+    <t>Seo Herin</t>
+  </si>
+  <si>
+    <t>Shin Sia</t>
+  </si>
+  <si>
+    <t>Bae Eun Yeong</t>
+  </si>
+  <si>
+    <t>Jang Gyuri</t>
+  </si>
+  <si>
+    <t>Chu Won Hui</t>
+  </si>
+  <si>
+    <t>Park So Myeong</t>
+  </si>
+  <si>
+    <t>Lee Yeong Yoo</t>
+  </si>
+  <si>
+    <t>Lee Hae In</t>
+  </si>
+  <si>
+    <t>Hong Si Woo</t>
+  </si>
+  <si>
+    <t>Jo Se Lim</t>
+  </si>
+  <si>
+    <t>Jo Yuri</t>
+  </si>
+  <si>
+    <t>Baek Ji Heon</t>
+  </si>
+  <si>
+    <t>Jenny / Kim Joo Hyun</t>
+  </si>
+  <si>
+    <t>Lee Na Gyung</t>
+  </si>
+  <si>
+    <t>Jessica Lee</t>
+  </si>
+  <si>
+    <t>Yoon Ji Woo</t>
+  </si>
+  <si>
+    <t>Kim Eun Kyul</t>
+  </si>
+  <si>
+    <t>Jo Young Ju</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>She lost her voice during the singing part.</t>
+  </si>
+  <si>
+    <t>Physical should be 6.2, not 3.5.</t>
+  </si>
+  <si>
+    <t>Vocal</t>
+  </si>
+  <si>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -296,10 +404,10 @@
     <tableColumn id="1" xr3:uid="{A58BC3CF-2122-4E00-B72A-FD2DD1E9E6D5}" name="Chinese_Name"/>
     <tableColumn id="2" xr3:uid="{C2C7527B-3BF9-4FD4-841C-8D6B6B4E4FB8}" name="English_Name"/>
     <tableColumn id="3" xr3:uid="{8C7118E1-8C77-4E01-9EB4-CA83871872DA}" name="Date_of_Birth"/>
-    <tableColumn id="4" xr3:uid="{5D4ECA23-2741-44E8-BDA9-A9FD95D22933}" name="Vocal_Rating"/>
-    <tableColumn id="5" xr3:uid="{7F9E5508-9D0C-4CA7-B416-7AD50FA2FB2C}" name="Dance_Rating"/>
-    <tableColumn id="6" xr3:uid="{2F08C1B6-D988-4F53-A894-2FB62798C21D}" name="Physical_Rating"/>
-    <tableColumn id="7" xr3:uid="{5F0A4D68-3DAE-4858-BEB9-64B94E649DB0}" name="Overall_Rating"/>
+    <tableColumn id="4" xr3:uid="{5D4ECA23-2741-44E8-BDA9-A9FD95D22933}" name="Vocal"/>
+    <tableColumn id="5" xr3:uid="{7F9E5508-9D0C-4CA7-B416-7AD50FA2FB2C}" name="Dance"/>
+    <tableColumn id="6" xr3:uid="{2F08C1B6-D988-4F53-A894-2FB62798C21D}" name="Physical"/>
+    <tableColumn id="7" xr3:uid="{5F0A4D68-3DAE-4858-BEB9-64B94E649DB0}" name="Overall"/>
     <tableColumn id="8" xr3:uid="{F65C0D17-909C-46CB-927D-939E0CEA2166}" name="Basic_Strength_Ranking"/>
     <tableColumn id="9" xr3:uid="{6F48FB8E-8E0D-43BE-A400-3699F2EB1A3A}" name="Final_Ranking"/>
     <tableColumn id="10" xr3:uid="{5FDF561D-01D0-4E56-9E88-A9B1D1C3426E}" name="Round_Eliminated"/>
@@ -630,22 +738,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
     <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
     <col min="8" max="8" width="22.08984375" customWidth="1"/>
     <col min="9" max="9" width="13.90625" customWidth="1"/>
     <col min="10" max="10" width="17.26953125" customWidth="1"/>
-    <col min="11" max="11" width="29.26953125" customWidth="1"/>
+    <col min="11" max="11" width="35.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -656,39 +764,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>37406</v>
@@ -712,18 +820,18 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>34253</v>
@@ -747,18 +855,18 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>36660</v>
@@ -782,15 +890,15 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>35702</v>
@@ -814,15 +922,15 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>36844</v>
@@ -846,15 +954,15 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>35712</v>
@@ -878,23 +986,59 @@
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1">
+        <v>35791</v>
+      </c>
+      <c r="D8">
+        <v>7.2</v>
+      </c>
+      <c r="E8">
+        <v>7.1</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7.1</v>
       </c>
       <c r="H8">
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1">
+        <v>38132</v>
+      </c>
+      <c r="D9">
+        <v>9.5</v>
+      </c>
+      <c r="E9">
+        <v>6.1</v>
+      </c>
+      <c r="F9">
+        <v>5.5</v>
+      </c>
+      <c r="G9">
+        <v>7.03</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -902,7 +1046,25 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1">
+        <v>35487</v>
+      </c>
+      <c r="D10">
+        <v>5.8</v>
+      </c>
+      <c r="E10">
+        <v>6.2</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
       </c>
       <c r="H10">
         <v>9</v>
@@ -910,7 +1072,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1">
+        <v>35200</v>
+      </c>
+      <c r="D11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>6.4</v>
+      </c>
+      <c r="G11">
+        <v>6.9</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -918,15 +1098,57 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1">
+        <v>36122</v>
+      </c>
+      <c r="D12">
+        <v>6.5</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>6.5</v>
+      </c>
+      <c r="G12">
+        <v>6.67</v>
       </c>
       <c r="H12">
         <v>11</v>
       </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="1">
+        <v>35573</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F13">
+        <v>3.5</v>
+      </c>
+      <c r="G13">
+        <v>6.6</v>
       </c>
       <c r="H13">
         <v>12</v>
@@ -934,15 +1156,60 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="1">
+        <v>35874</v>
+      </c>
+      <c r="D14">
+        <v>7.9</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>6.2</v>
+      </c>
+      <c r="G14">
+        <v>6.37</v>
       </c>
       <c r="H14">
         <v>13</v>
       </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1">
+        <v>36442</v>
+      </c>
+      <c r="D15">
+        <v>5.9</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>6.3</v>
       </c>
       <c r="H15">
         <v>14</v>
@@ -950,138 +1217,441 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1">
+        <v>35437</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F16">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G16">
+        <v>6.27</v>
       </c>
       <c r="H16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="1">
+        <v>36264</v>
+      </c>
+      <c r="D17">
+        <v>5.7</v>
+      </c>
+      <c r="E17">
+        <v>7.4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>6.03</v>
       </c>
       <c r="H17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="1">
+        <v>35180</v>
+      </c>
+      <c r="D18">
+        <v>6.4</v>
+      </c>
+      <c r="E18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G18">
+        <v>5.4</v>
       </c>
       <c r="H18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1">
+        <v>36508</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>5.4</v>
+      </c>
+      <c r="F19">
+        <v>6.1</v>
+      </c>
+      <c r="G19">
+        <v>5.17</v>
       </c>
       <c r="H19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1">
+        <v>36547</v>
+      </c>
+      <c r="D20">
+        <v>6.1</v>
+      </c>
+      <c r="E20">
+        <v>6.3</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>4.8</v>
       </c>
       <c r="H20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="1">
+        <v>35067</v>
+      </c>
+      <c r="D21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E21">
+        <v>7.5</v>
+      </c>
+      <c r="F21">
+        <v>1.6</v>
+      </c>
+      <c r="G21">
+        <v>4.67</v>
       </c>
       <c r="H21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="1">
+        <v>37313</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>5.5</v>
+      </c>
+      <c r="F22">
+        <v>2.4</v>
+      </c>
+      <c r="G22">
+        <v>4.63</v>
       </c>
       <c r="H22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1">
+        <v>36336</v>
+      </c>
+      <c r="D23">
+        <v>5.6</v>
+      </c>
+      <c r="E23">
+        <v>5.6</v>
+      </c>
+      <c r="F23">
+        <v>1.5</v>
+      </c>
+      <c r="G23">
+        <v>4.2300000000000004</v>
       </c>
       <c r="H23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1">
+        <v>35471</v>
+      </c>
+      <c r="D24">
+        <v>4.2</v>
+      </c>
+      <c r="E24">
+        <v>5.3</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>4.17</v>
       </c>
       <c r="H24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1">
+        <v>35986</v>
+      </c>
+      <c r="D25">
+        <v>3.5</v>
+      </c>
+      <c r="E25">
+        <v>5.7</v>
+      </c>
+      <c r="F25">
+        <v>2.9</v>
+      </c>
+      <c r="G25">
+        <v>4.03</v>
       </c>
       <c r="H25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="1">
+        <v>34519</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>8.4</v>
+      </c>
+      <c r="F26">
+        <v>1.8</v>
+      </c>
+      <c r="G26">
+        <v>3.73</v>
       </c>
       <c r="H26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="1">
+        <v>35489</v>
+      </c>
+      <c r="D27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>3.2</v>
+      </c>
+      <c r="G27">
+        <v>3.53</v>
       </c>
       <c r="H27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="1">
+        <v>36664</v>
+      </c>
+      <c r="D28">
+        <v>4.3</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>2.1</v>
+      </c>
+      <c r="G28">
+        <v>3.47</v>
       </c>
       <c r="H28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="C29" s="1">
+        <v>38026</v>
+      </c>
+      <c r="D29">
+        <v>4.5</v>
+      </c>
+      <c r="E29">
+        <v>4.5</v>
+      </c>
+      <c r="F29">
+        <v>1.2</v>
+      </c>
+      <c r="G29">
+        <v>3.4</v>
       </c>
       <c r="H29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="1">
+        <v>37728</v>
+      </c>
+      <c r="D30">
+        <v>1.2</v>
+      </c>
+      <c r="E30">
+        <v>5.8</v>
+      </c>
+      <c r="F30">
+        <v>2.7</v>
+      </c>
+      <c r="G30">
+        <v>3.23</v>
       </c>
       <c r="H30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1">
+        <v>37186</v>
       </c>
       <c r="H31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="1">
+        <v>37436</v>
       </c>
       <c r="H32">
         <v>31</v>
@@ -1089,7 +1659,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="1">
+        <v>36678</v>
       </c>
       <c r="H33">
         <v>32</v>
@@ -1097,7 +1673,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1">
+        <v>36932</v>
       </c>
       <c r="H34">
         <v>33</v>
@@ -1105,7 +1687,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="1">
+        <v>37069</v>
       </c>
       <c r="H35">
         <v>34</v>
@@ -1113,7 +1701,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="1">
+        <v>38363</v>
       </c>
       <c r="H36">
         <v>35</v>
@@ -1121,7 +1715,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="1">
+        <v>34923</v>
       </c>
       <c r="H37">
         <v>36</v>
@@ -1129,42 +1729,84 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="C38" s="1">
+        <v>35340</v>
       </c>
       <c r="H38">
         <v>37</v>
       </c>
+      <c r="J38" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1">
+        <v>35455</v>
       </c>
       <c r="H39">
         <v>38</v>
       </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="1">
+        <v>36216</v>
       </c>
       <c r="H40">
         <v>39</v>
       </c>
+      <c r="J40" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="1">
+        <v>36240</v>
       </c>
       <c r="H41">
         <v>40</v>
       </c>
+      <c r="J41" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="1">
+        <v>35396</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1185,10 +1827,10 @@
         <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K42" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Idol School data entry complete
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49764788-8856-4E82-BC00-BFB1C0FB631A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413ED440-B2F8-4CCB-8DEE-F6E559012026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
   <sheets>
     <sheet name="Idol_School_Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Produce_48_Dataset" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="119">
   <si>
     <t>Chinese_Name</t>
   </si>
@@ -152,9 +153,6 @@
     <t>徐慧仁</t>
   </si>
   <si>
-    <t>申知恩</t>
-  </si>
-  <si>
     <t>朴昭名</t>
   </si>
   <si>
@@ -221,9 +219,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Left the show due to health issues</t>
-  </si>
-  <si>
     <t>Park Sun</t>
   </si>
   <si>
@@ -326,12 +321,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>She lost her voice during the singing part.</t>
-  </si>
-  <si>
-    <t>Physical should be 6.2, not 3.5.</t>
-  </si>
-  <si>
     <t>Vocal</t>
   </si>
   <si>
@@ -342,14 +331,85 @@
   </si>
   <si>
     <t>Overall</t>
+  </si>
+  <si>
+    <t>Vocal: She lost her voice during the singing part.</t>
+  </si>
+  <si>
+    <t>Originally from Taiwan.</t>
+  </si>
+  <si>
+    <t>Left the show due to health issues.</t>
+  </si>
+  <si>
+    <t>Physical should be 6.2, not 3.5. (according to the video screenshot)</t>
+  </si>
+  <si>
+    <t>Dance: The teacher assigned Bae Eun Yeong to help Yoo Ji Na learn.</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>申詩雅</t>
+  </si>
+  <si>
+    <t>First_Eval</t>
+  </si>
+  <si>
+    <t>Second_Eval</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>張員瑛</t>
+  </si>
+  <si>
+    <t>Jang Won Young</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>宮脇咲良</t>
+  </si>
+  <si>
+    <t>Miyawaki Sakura</t>
+  </si>
+  <si>
+    <t>矢吹奈子</t>
+  </si>
+  <si>
+    <t>Yabuki Nako</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -365,7 +425,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,13 +433,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,9 +808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,7 +825,7 @@
     <col min="8" max="8" width="22.08984375" customWidth="1"/>
     <col min="9" max="9" width="13.90625" customWidth="1"/>
     <col min="10" max="10" width="17.26953125" customWidth="1"/>
-    <col min="11" max="11" width="35.26953125" customWidth="1"/>
+    <col min="11" max="11" width="56.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -767,16 +839,16 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -994,7 +1066,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1">
         <v>35791</v>
@@ -1013,6 +1085,9 @@
       </c>
       <c r="H8">
         <v>7</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
@@ -1023,7 +1098,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1">
         <v>38132</v>
@@ -1042,6 +1117,12 @@
       </c>
       <c r="H9">
         <v>8</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1049,7 +1130,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
         <v>35487</v>
@@ -1068,6 +1149,12 @@
       </c>
       <c r="H10">
         <v>9</v>
+      </c>
+      <c r="I10">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1075,7 +1162,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1">
         <v>35200</v>
@@ -1094,6 +1181,12 @@
       </c>
       <c r="H11">
         <v>10</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1101,7 +1194,7 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1">
         <v>36122</v>
@@ -1133,7 +1226,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1">
         <v>35573</v>
@@ -1152,6 +1245,12 @@
       </c>
       <c r="H13">
         <v>12</v>
+      </c>
+      <c r="I13">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1159,7 +1258,7 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1">
         <v>35874</v>
@@ -1186,7 +1285,7 @@
         <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1194,7 +1293,7 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1">
         <v>36442</v>
@@ -1213,6 +1312,12 @@
       </c>
       <c r="H15">
         <v>14</v>
+      </c>
+      <c r="I15">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1220,7 +1325,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1">
         <v>35437</v>
@@ -1252,7 +1357,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1">
         <v>36264</v>
@@ -1271,6 +1376,12 @@
       </c>
       <c r="H17">
         <v>16</v>
+      </c>
+      <c r="I17">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1278,7 +1389,7 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1">
         <v>35180</v>
@@ -1297,6 +1408,12 @@
       </c>
       <c r="H18">
         <v>17</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1304,7 +1421,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1">
         <v>36508</v>
@@ -1323,6 +1440,12 @@
       </c>
       <c r="H19">
         <v>18</v>
+      </c>
+      <c r="I19">
+        <v>17</v>
+      </c>
+      <c r="J19" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1330,7 +1453,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1">
         <v>36547</v>
@@ -1349,6 +1472,9 @@
       </c>
       <c r="H20">
         <v>19</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
       </c>
       <c r="J20" t="s">
         <v>14</v>
@@ -1359,7 +1485,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1">
         <v>35067</v>
@@ -1378,6 +1504,12 @@
       </c>
       <c r="H21">
         <v>20</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1385,7 +1517,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1">
         <v>37313</v>
@@ -1405,13 +1537,19 @@
       <c r="H22">
         <v>21</v>
       </c>
+      <c r="I22">
+        <v>22</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1">
         <v>36336</v>
@@ -1431,13 +1569,19 @@
       <c r="H23">
         <v>22</v>
       </c>
+      <c r="I23">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1">
         <v>35471</v>
@@ -1457,13 +1601,19 @@
       <c r="H24">
         <v>23</v>
       </c>
+      <c r="I24">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1">
         <v>35986</v>
@@ -1483,13 +1633,19 @@
       <c r="H25">
         <v>24</v>
       </c>
+      <c r="I25">
+        <v>32</v>
+      </c>
+      <c r="J25" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1">
         <v>34519</v>
@@ -1516,15 +1672,15 @@
         <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="1">
         <v>35489</v>
@@ -1544,13 +1700,19 @@
       <c r="H27">
         <v>26</v>
       </c>
+      <c r="I27">
+        <v>39</v>
+      </c>
+      <c r="J27" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1">
         <v>36664</v>
@@ -1570,13 +1732,19 @@
       <c r="H28">
         <v>27</v>
       </c>
+      <c r="I28">
+        <v>40</v>
+      </c>
+      <c r="J28" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1">
         <v>38026</v>
@@ -1596,13 +1764,19 @@
       <c r="H29">
         <v>28</v>
       </c>
+      <c r="I29">
+        <v>34</v>
+      </c>
+      <c r="J29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1">
         <v>37728</v>
@@ -1631,129 +1805,285 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1">
         <v>37186</v>
       </c>
+      <c r="D31">
+        <v>1.3</v>
+      </c>
+      <c r="E31">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F31">
+        <v>5.9</v>
+      </c>
+      <c r="G31">
+        <v>3.13</v>
+      </c>
       <c r="H31">
         <v>30</v>
       </c>
+      <c r="I31">
+        <v>15</v>
+      </c>
+      <c r="J31" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1">
         <v>37436</v>
       </c>
+      <c r="D32">
+        <v>3.3</v>
+      </c>
+      <c r="E32">
+        <v>4.2</v>
+      </c>
+      <c r="F32">
+        <v>1.7</v>
+      </c>
+      <c r="G32">
+        <v>3.07</v>
+      </c>
       <c r="H32">
         <v>31</v>
       </c>
+      <c r="I32">
+        <v>28</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1">
         <v>36678</v>
       </c>
+      <c r="D33">
+        <v>2.1</v>
+      </c>
+      <c r="E33">
+        <v>3.2</v>
+      </c>
+      <c r="F33">
+        <v>3.3</v>
+      </c>
+      <c r="G33">
+        <v>2.87</v>
+      </c>
       <c r="H33">
         <v>32</v>
       </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="1">
         <v>36932</v>
       </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>3.9</v>
+      </c>
+      <c r="F34">
+        <v>1.2</v>
+      </c>
+      <c r="G34">
+        <v>2.7</v>
+      </c>
       <c r="H34">
         <v>33</v>
       </c>
+      <c r="I34">
+        <v>35</v>
+      </c>
+      <c r="J34" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1">
         <v>37069</v>
       </c>
+      <c r="D35">
+        <v>3.4</v>
+      </c>
+      <c r="E35">
+        <v>3.6</v>
+      </c>
+      <c r="F35">
+        <v>0.6</v>
+      </c>
+      <c r="G35">
+        <v>2.5299999999999998</v>
+      </c>
       <c r="H35">
         <v>34</v>
       </c>
+      <c r="I35">
+        <v>37</v>
+      </c>
+      <c r="J35" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1">
         <v>38363</v>
       </c>
+      <c r="D36">
+        <v>1.4</v>
+      </c>
+      <c r="E36">
+        <v>3.5</v>
+      </c>
+      <c r="F36">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G36">
+        <v>2.4</v>
+      </c>
       <c r="H36">
         <v>35</v>
       </c>
+      <c r="I36">
+        <v>31</v>
+      </c>
+      <c r="J36" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37" s="1">
         <v>34923</v>
       </c>
+      <c r="D37">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E37">
+        <v>3.1</v>
+      </c>
+      <c r="F37">
+        <v>0.8</v>
+      </c>
+      <c r="G37">
+        <v>2.0299999999999998</v>
+      </c>
       <c r="H37">
         <v>36</v>
       </c>
+      <c r="I37">
+        <v>25</v>
+      </c>
+      <c r="J37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
         <v>54</v>
-      </c>
-      <c r="B38" t="s">
-        <v>55</v>
       </c>
       <c r="C38" s="1">
         <v>35340</v>
       </c>
+      <c r="D38">
+        <v>2.5</v>
+      </c>
+      <c r="E38">
+        <v>2.6</v>
+      </c>
+      <c r="F38">
+        <v>0.7</v>
+      </c>
+      <c r="G38">
+        <v>1.93</v>
+      </c>
       <c r="H38">
         <v>37</v>
       </c>
+      <c r="I38">
+        <v>33</v>
+      </c>
       <c r="J38" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="K38" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="1">
         <v>35455</v>
       </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>3.3</v>
+      </c>
+      <c r="F39">
+        <v>0.4</v>
+      </c>
+      <c r="G39">
+        <v>1.9</v>
+      </c>
       <c r="H39">
         <v>38</v>
       </c>
@@ -1763,47 +2093,80 @@
       <c r="J39" t="s">
         <v>7</v>
       </c>
+      <c r="K39" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1">
         <v>36216</v>
       </c>
+      <c r="D40">
+        <v>1.5</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1.5</v>
+      </c>
       <c r="H40">
         <v>39</v>
       </c>
+      <c r="I40">
+        <v>16</v>
+      </c>
       <c r="J40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="1">
         <v>36240</v>
       </c>
+      <c r="D41">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0.9</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
       <c r="H41">
         <v>40</v>
       </c>
+      <c r="I41">
+        <v>36</v>
+      </c>
       <c r="J41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1">
         <v>35396</v>
@@ -1827,10 +2190,10 @@
         <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K42" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1839,4 +2202,296 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="1">
+        <v>38230</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="1">
+        <v>35873</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="1">
+        <v>37186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1">
+        <v>37060</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
initial data cleaning for Idol School
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413ED440-B2F8-4CCB-8DEE-F6E559012026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB287FED-CD35-4951-99A5-34248A499F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
@@ -39,18 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="119">
   <si>
-    <t>Chinese_Name</t>
-  </si>
-  <si>
-    <t>English_Name</t>
-  </si>
-  <si>
-    <t>Basic_Strength_Ranking</t>
-  </si>
-  <si>
-    <t>Final_Ranking</t>
-  </si>
-  <si>
     <t>Round_Eliminated</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
     <t>Survived</t>
   </si>
   <si>
-    <t>Date_of_Birth</t>
-  </si>
-  <si>
     <t>宋河英</t>
   </si>
   <si>
@@ -394,6 +379,21 @@
   </si>
   <si>
     <t>Yabuki Nako</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Name_Chn</t>
+  </si>
+  <si>
+    <t>Name_Eng</t>
+  </si>
+  <si>
+    <t>Ability_Rank</t>
+  </si>
+  <si>
+    <t>Final_Rank</t>
   </si>
 </sst>
 </file>
@@ -473,15 +473,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7635057D-705D-4C46-B283-D8737736A85F}" name="Table1" displayName="Table1" ref="A1:K42" totalsRowShown="0">
   <autoFilter ref="A1:K42" xr:uid="{7635057D-705D-4C46-B283-D8737736A85F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{A58BC3CF-2122-4E00-B72A-FD2DD1E9E6D5}" name="Chinese_Name"/>
-    <tableColumn id="2" xr3:uid="{C2C7527B-3BF9-4FD4-841C-8D6B6B4E4FB8}" name="English_Name"/>
-    <tableColumn id="3" xr3:uid="{8C7118E1-8C77-4E01-9EB4-CA83871872DA}" name="Date_of_Birth"/>
+    <tableColumn id="1" xr3:uid="{A58BC3CF-2122-4E00-B72A-FD2DD1E9E6D5}" name="Name_Chn"/>
+    <tableColumn id="2" xr3:uid="{C2C7527B-3BF9-4FD4-841C-8D6B6B4E4FB8}" name="Name_Eng"/>
+    <tableColumn id="3" xr3:uid="{8C7118E1-8C77-4E01-9EB4-CA83871872DA}" name="DOB"/>
     <tableColumn id="4" xr3:uid="{5D4ECA23-2741-44E8-BDA9-A9FD95D22933}" name="Vocal"/>
     <tableColumn id="5" xr3:uid="{7F9E5508-9D0C-4CA7-B416-7AD50FA2FB2C}" name="Dance"/>
     <tableColumn id="6" xr3:uid="{2F08C1B6-D988-4F53-A894-2FB62798C21D}" name="Physical"/>
     <tableColumn id="7" xr3:uid="{5F0A4D68-3DAE-4858-BEB9-64B94E649DB0}" name="Overall"/>
-    <tableColumn id="8" xr3:uid="{F65C0D17-909C-46CB-927D-939E0CEA2166}" name="Basic_Strength_Ranking"/>
-    <tableColumn id="9" xr3:uid="{6F48FB8E-8E0D-43BE-A400-3699F2EB1A3A}" name="Final_Ranking"/>
+    <tableColumn id="8" xr3:uid="{F65C0D17-909C-46CB-927D-939E0CEA2166}" name="Ability_Rank"/>
+    <tableColumn id="9" xr3:uid="{6F48FB8E-8E0D-43BE-A400-3699F2EB1A3A}" name="Final_Rank"/>
     <tableColumn id="10" xr3:uid="{5FDF561D-01D0-4E56-9E88-A9B1D1C3426E}" name="Round_Eliminated"/>
     <tableColumn id="11" xr3:uid="{DC5B0B4A-57F6-42E4-822B-CF800F93543A}" name="Special_Notes"/>
   </tableColumns>
@@ -808,9 +808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C31" sqref="C31"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,45 +830,45 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>37406</v>
@@ -892,18 +892,18 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>34253</v>
@@ -927,18 +927,18 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>36660</v>
@@ -962,15 +962,15 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>35702</v>
@@ -994,15 +994,15 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>36844</v>
@@ -1026,15 +1026,15 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>35712</v>
@@ -1058,15 +1058,15 @@
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1">
         <v>35791</v>
@@ -1090,15 +1090,15 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1">
         <v>38132</v>
@@ -1122,15 +1122,15 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1">
         <v>35487</v>
@@ -1154,15 +1154,15 @@
         <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1">
         <v>35200</v>
@@ -1186,15 +1186,15 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1">
         <v>36122</v>
@@ -1218,15 +1218,15 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1">
         <v>35573</v>
@@ -1250,15 +1250,15 @@
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1">
         <v>35874</v>
@@ -1282,18 +1282,18 @@
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1">
         <v>36442</v>
@@ -1317,15 +1317,15 @@
         <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <v>35437</v>
@@ -1349,15 +1349,15 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1">
         <v>36264</v>
@@ -1381,15 +1381,15 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1">
         <v>35180</v>
@@ -1413,15 +1413,15 @@
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1">
         <v>36508</v>
@@ -1445,15 +1445,15 @@
         <v>17</v>
       </c>
       <c r="J19" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1">
         <v>36547</v>
@@ -1477,15 +1477,15 @@
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1">
         <v>35067</v>
@@ -1509,15 +1509,15 @@
         <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1">
         <v>37313</v>
@@ -1541,15 +1541,15 @@
         <v>22</v>
       </c>
       <c r="J22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1">
         <v>36336</v>
@@ -1573,15 +1573,15 @@
         <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1">
         <v>35471</v>
@@ -1605,15 +1605,15 @@
         <v>12</v>
       </c>
       <c r="J24" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1">
         <v>35986</v>
@@ -1637,15 +1637,15 @@
         <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1">
         <v>34519</v>
@@ -1669,18 +1669,18 @@
         <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1">
         <v>35489</v>
@@ -1704,15 +1704,15 @@
         <v>39</v>
       </c>
       <c r="J27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1">
         <v>36664</v>
@@ -1736,15 +1736,15 @@
         <v>40</v>
       </c>
       <c r="J28" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1">
         <v>38026</v>
@@ -1768,15 +1768,15 @@
         <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1">
         <v>37728</v>
@@ -1800,15 +1800,15 @@
         <v>8</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C31" s="1">
         <v>37186</v>
@@ -1832,15 +1832,15 @@
         <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1">
         <v>37436</v>
@@ -1864,15 +1864,15 @@
         <v>28</v>
       </c>
       <c r="J32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1">
         <v>36678</v>
@@ -1896,15 +1896,15 @@
         <v>5</v>
       </c>
       <c r="J33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1">
         <v>36932</v>
@@ -1928,15 +1928,15 @@
         <v>35</v>
       </c>
       <c r="J34" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1">
         <v>37069</v>
@@ -1960,15 +1960,15 @@
         <v>37</v>
       </c>
       <c r="J35" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1">
         <v>38363</v>
@@ -1992,15 +1992,15 @@
         <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1">
         <v>34923</v>
@@ -2024,15 +2024,15 @@
         <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1">
         <v>35340</v>
@@ -2056,18 +2056,18 @@
         <v>33</v>
       </c>
       <c r="J38" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K38" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1">
         <v>35455</v>
@@ -2091,18 +2091,18 @@
         <v>10</v>
       </c>
       <c r="J39" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1">
         <v>36216</v>
@@ -2126,15 +2126,15 @@
         <v>16</v>
       </c>
       <c r="J40" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C41" s="1">
         <v>36240</v>
@@ -2158,15 +2158,15 @@
         <v>36</v>
       </c>
       <c r="J41" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1">
         <v>35396</v>
@@ -2190,10 +2190,10 @@
         <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K42" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2209,7 +2209,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2226,228 +2226,228 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1">
         <v>38230</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1">
         <v>35873</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1">
         <v>37186</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1">
         <v>37060</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G12">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G13">
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G15">
         <v>14</v>

</xml_diff>

<commit_message>
corrected another score from the sorting  process
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB287FED-CD35-4951-99A5-34248A499F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522BF3BF-BD2B-4E29-9719-74D69D17398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
   <sheets>
     <sheet name="Idol_School_Dataset" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
   <si>
     <t>Round_Eliminated</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Left the show due to health issues.</t>
   </si>
   <si>
-    <t>Physical should be 6.2, not 3.5. (according to the video screenshot)</t>
-  </si>
-  <si>
     <t>Dance: The teacher assigned Bae Eun Yeong to help Yoo Ji Na learn.</t>
   </si>
   <si>
@@ -394,6 +391,12 @@
   </si>
   <si>
     <t>Final_Rank</t>
+  </si>
+  <si>
+    <t>Physical should be 6.2, not 3.5. (according to the video screenshots)</t>
+  </si>
+  <si>
+    <t>Physical should be 1.3, not 1.2. (according to the video screenshots)</t>
   </si>
 </sst>
 </file>
@@ -808,9 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,13 +833,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>116</v>
-      </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
         <v>89</v>
@@ -851,10 +854,10 @@
         <v>92</v>
       </c>
       <c r="H1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" t="s">
         <v>117</v>
-      </c>
-      <c r="I1" t="s">
-        <v>118</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1122,7 +1125,7 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1285,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1317,7 +1320,7 @@
         <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1546,7 +1549,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
         <v>71</v>
@@ -1637,7 +1640,7 @@
         <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -1756,10 +1759,10 @@
         <v>4.5</v>
       </c>
       <c r="F29">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="G29">
-        <v>3.4</v>
+        <v>3.43</v>
       </c>
       <c r="H29">
         <v>28</v>
@@ -1769,6 +1772,9 @@
       </c>
       <c r="J29" t="s">
         <v>88</v>
+      </c>
+      <c r="K29" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -1992,7 +1998,7 @@
         <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -2094,7 +2100,7 @@
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -2208,7 +2214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -2226,25 +2232,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -2255,22 +2261,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
         <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>106</v>
       </c>
       <c r="C2" s="1">
         <v>38230</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2281,22 +2287,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
         <v>110</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
       </c>
       <c r="C3" s="1">
         <v>35873</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2316,13 +2322,13 @@
         <v>37186</v>
       </c>
       <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
         <v>108</v>
       </c>
-      <c r="E4" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -2333,7 +2339,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2344,7 +2350,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -2355,22 +2361,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
       </c>
       <c r="C7" s="1">
         <v>37060</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -2381,7 +2387,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -2392,7 +2398,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -2403,7 +2409,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -2414,7 +2420,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -2425,7 +2431,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -2436,7 +2442,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -2447,7 +2453,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -2455,7 +2461,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15">
         <v>14</v>

</xml_diff>

<commit_message>
continued data entry for Produce 48 (2018)
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522BF3BF-BD2B-4E29-9719-74D69D17398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAAEC1-4DEC-4B1B-97E3-0E072C126BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
   <sheets>
     <sheet name="Idol_School_Dataset" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="148">
   <si>
     <t>Round_Eliminated</t>
   </si>
@@ -397,13 +397,97 @@
   </si>
   <si>
     <t>Physical should be 1.3, not 1.2. (according to the video screenshots)</t>
+  </si>
+  <si>
+    <t>崔叡娜</t>
+  </si>
+  <si>
+    <t>Choi Ye Na</t>
+  </si>
+  <si>
+    <t>An Yu Jin</t>
+  </si>
+  <si>
+    <t>安俞真</t>
+  </si>
+  <si>
+    <t>權恩妃</t>
+  </si>
+  <si>
+    <t>Kwon Eun Bi</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Kang Hye Won</t>
+  </si>
+  <si>
+    <t>姜惠元</t>
+  </si>
+  <si>
+    <t>Kim Chae Won</t>
+  </si>
+  <si>
+    <t>金采源</t>
+  </si>
+  <si>
+    <t>Kim Min Ju</t>
+  </si>
+  <si>
+    <t>金玟周</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Lee Chae Yeon</t>
+  </si>
+  <si>
+    <t>李彩演</t>
+  </si>
+  <si>
+    <t>Han Cho Won</t>
+  </si>
+  <si>
+    <t>韓霄瑗</t>
+  </si>
+  <si>
+    <t>李佳恩</t>
+  </si>
+  <si>
+    <t>Lee Ka Eun</t>
+  </si>
+  <si>
+    <t>Honda Hitomi</t>
+  </si>
+  <si>
+    <t>本田仁美</t>
+  </si>
+  <si>
+    <t>Miyazaki Miho</t>
+  </si>
+  <si>
+    <t>宮崎美穂</t>
+  </si>
+  <si>
+    <t>Originally ranked 5th, but the organized modified her ranking to 14th.</t>
+  </si>
+  <si>
+    <t>Originally ranked 6th, but the organized modified her ranking to 13th.</t>
+  </si>
+  <si>
+    <t>朴海允</t>
+  </si>
+  <si>
+    <t>Park Hae Yoon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +499,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -811,9 +901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K29" sqref="K29"/>
+      <selection pane="topRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2212,22 +2302,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.90625" customWidth="1"/>
     <col min="3" max="3" width="13.36328125" customWidth="1"/>
     <col min="4" max="4" width="9.7265625" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="16.36328125" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" customWidth="1"/>
+    <col min="9" max="9" width="58.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -2338,6 +2429,21 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36432</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>106</v>
+      </c>
       <c r="F5" t="s">
         <v>102</v>
       </c>
@@ -2349,6 +2455,21 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="1">
+        <v>37865</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
       <c r="F6" t="s">
         <v>102</v>
       </c>
@@ -2386,6 +2507,21 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="1">
+        <v>34969</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
       <c r="F8" t="s">
         <v>102</v>
       </c>
@@ -2397,6 +2533,21 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="1">
+        <v>36346</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
       <c r="F9" t="s">
         <v>102</v>
       </c>
@@ -2408,6 +2559,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="1">
+        <v>37170</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
       <c r="F10" t="s">
         <v>103</v>
       </c>
@@ -2419,6 +2585,21 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="1">
+        <v>36739</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
       <c r="F11" t="s">
         <v>102</v>
       </c>
@@ -2430,6 +2611,21 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="1">
+        <v>36927</v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>126</v>
+      </c>
       <c r="F12" t="s">
         <v>102</v>
       </c>
@@ -2441,6 +2637,21 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="1">
+        <v>36536</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
       <c r="F13" t="s">
         <v>102</v>
       </c>
@@ -2452,52 +2663,419 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="1">
+        <v>37515</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
+        <v>106</v>
+      </c>
       <c r="F14" t="s">
         <v>102</v>
       </c>
       <c r="G14">
         <v>13</v>
       </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="1">
+        <v>34566</v>
+      </c>
+      <c r="D15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" t="s">
+        <v>107</v>
+      </c>
       <c r="F15" t="s">
         <v>102</v>
       </c>
       <c r="G15">
         <v>14</v>
       </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="1">
+        <v>34180</v>
+      </c>
+      <c r="D16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" t="s">
+        <v>103</v>
+      </c>
       <c r="G16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>103</v>
+      </c>
       <c r="G17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
       <c r="G18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
       <c r="G19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="1">
+        <v>35074</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>102</v>
+      </c>
       <c r="G20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>103</v>
+      </c>
       <c r="G21">
         <v>20</v>
       </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1">
+        <v>36216</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>34</v>
+      </c>
+      <c r="H35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>35</v>
+      </c>
+      <c r="H36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>36</v>
+      </c>
+      <c r="H37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>37</v>
+      </c>
+      <c r="H38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more datapoints to Produce 48
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAAEC1-4DEC-4B1B-97E3-0E072C126BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB9FFCC-9A4C-4864-B98F-D39287170652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="181">
   <si>
     <t>Round_Eliminated</t>
   </si>
@@ -57,12 +57,6 @@
     <t>劉怡伶</t>
   </si>
   <si>
-    <t>Originally from Thailand</t>
-  </si>
-  <si>
-    <t>Originally from Singapore</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -481,6 +475,111 @@
   </si>
   <si>
     <t>Park Hae Yoon</t>
+  </si>
+  <si>
+    <t>高橋朱里</t>
+  </si>
+  <si>
+    <t>Takahashi Juri</t>
+  </si>
+  <si>
+    <t>竹内美宥</t>
+  </si>
+  <si>
+    <t>Takeuchi Miyu</t>
+  </si>
+  <si>
+    <t>下尾美羽</t>
+  </si>
+  <si>
+    <t>Shitao Miu</t>
+  </si>
+  <si>
+    <t>白間美瑠</t>
+  </si>
+  <si>
+    <t>Shiroma Miru</t>
+  </si>
+  <si>
+    <t>村瀨紗英</t>
+  </si>
+  <si>
+    <t>Murase Sae</t>
+  </si>
+  <si>
+    <t>後藤萌咲</t>
+  </si>
+  <si>
+    <t>Gotou Moe</t>
+  </si>
+  <si>
+    <t>金娜英</t>
+  </si>
+  <si>
+    <t>Kim Na Young</t>
+  </si>
+  <si>
+    <t>金鍍我</t>
+  </si>
+  <si>
+    <t>Kim Do Ah</t>
+  </si>
+  <si>
+    <t>許允真</t>
+  </si>
+  <si>
+    <t>Huh Yoon Jin</t>
+  </si>
+  <si>
+    <t>金施賢</t>
+  </si>
+  <si>
+    <t>Kim Si Hyeon</t>
+  </si>
+  <si>
+    <t>王怡人</t>
+  </si>
+  <si>
+    <t>Wang Yi Ren</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>羅高恩</t>
+  </si>
+  <si>
+    <t>Na Go Eun</t>
+  </si>
+  <si>
+    <t>高涖嘏</t>
+  </si>
+  <si>
+    <t>Ko Yu Jin</t>
+  </si>
+  <si>
+    <t>孫銀彩</t>
+  </si>
+  <si>
+    <t>Son Eun Chae</t>
+  </si>
+  <si>
+    <t>千葉惠里</t>
+  </si>
+  <si>
+    <t>小嶋真子</t>
+  </si>
+  <si>
+    <t>Matsui Jurina left the show while still in the top 58 ranking.</t>
+  </si>
+  <si>
+    <t>Originally from Thailand.</t>
+  </si>
+  <si>
+    <t>Originally from Singapore.</t>
+  </si>
+  <si>
+    <t>The only contestant from China.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +617,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -537,14 +636,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,9 +1012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G46" sqref="G46"/>
+      <selection pane="topRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,31 +1034,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>117</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -988,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1020,18 +1131,18 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>36660</v>
@@ -1055,15 +1166,15 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>35702</v>
@@ -1087,15 +1198,15 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>36844</v>
@@ -1124,10 +1235,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>35712</v>
@@ -1151,15 +1262,15 @@
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="1">
         <v>35791</v>
@@ -1183,15 +1294,15 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
         <v>38132</v>
@@ -1215,15 +1326,15 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>35487</v>
@@ -1247,15 +1358,15 @@
         <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>35200</v>
@@ -1279,15 +1390,15 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>36122</v>
@@ -1311,15 +1422,15 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1">
         <v>35573</v>
@@ -1348,10 +1459,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1">
         <v>35874</v>
@@ -1375,18 +1486,18 @@
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1">
         <v>36442</v>
@@ -1410,15 +1521,15 @@
         <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1">
         <v>35437</v>
@@ -1442,15 +1553,15 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1">
         <v>36264</v>
@@ -1474,15 +1585,15 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1">
         <v>35180</v>
@@ -1506,15 +1617,15 @@
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1">
         <v>36508</v>
@@ -1543,10 +1654,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1">
         <v>36547</v>
@@ -1570,15 +1681,15 @@
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1">
         <v>35067</v>
@@ -1602,15 +1713,15 @@
         <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1">
         <v>37313</v>
@@ -1634,15 +1745,15 @@
         <v>22</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1">
         <v>36336</v>
@@ -1666,15 +1777,15 @@
         <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1">
         <v>35471</v>
@@ -1703,10 +1814,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1">
         <v>35986</v>
@@ -1730,15 +1841,15 @@
         <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1">
         <v>34519</v>
@@ -1765,15 +1876,15 @@
         <v>3</v>
       </c>
       <c r="K26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1">
         <v>35489</v>
@@ -1797,15 +1908,15 @@
         <v>39</v>
       </c>
       <c r="J27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1">
         <v>36664</v>
@@ -1829,15 +1940,15 @@
         <v>40</v>
       </c>
       <c r="J28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
         <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
       </c>
       <c r="C29" s="1">
         <v>38026</v>
@@ -1861,18 +1972,18 @@
         <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1">
         <v>37728</v>
@@ -1896,15 +2007,15 @@
         <v>8</v>
       </c>
       <c r="J30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1">
         <v>37186</v>
@@ -1933,10 +2044,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1">
         <v>37436</v>
@@ -1960,15 +2071,15 @@
         <v>28</v>
       </c>
       <c r="J32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1">
         <v>36678</v>
@@ -1992,15 +2103,15 @@
         <v>5</v>
       </c>
       <c r="J33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1">
         <v>36932</v>
@@ -2024,15 +2135,15 @@
         <v>35</v>
       </c>
       <c r="J34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1">
         <v>37069</v>
@@ -2056,15 +2167,15 @@
         <v>37</v>
       </c>
       <c r="J35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1">
         <v>38363</v>
@@ -2088,15 +2199,15 @@
         <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="1">
         <v>34923</v>
@@ -2120,15 +2231,15 @@
         <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1">
         <v>35340</v>
@@ -2152,18 +2263,18 @@
         <v>33</v>
       </c>
       <c r="J38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1">
         <v>35455</v>
@@ -2190,15 +2301,15 @@
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1">
         <v>36216</v>
@@ -2227,10 +2338,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="1">
         <v>36240</v>
@@ -2254,15 +2365,15 @@
         <v>36</v>
       </c>
       <c r="J41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="1">
         <v>35396</v>
@@ -2286,10 +2397,10 @@
         <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2302,11 +2413,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I23" sqref="I23"/>
+      <selection pane="topRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2323,25 +2434,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
@@ -2352,334 +2463,335 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1">
         <v>38230</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1">
         <v>35873</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1">
         <v>37186</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1">
         <v>36432</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1">
         <v>37865</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1">
         <v>37060</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1">
         <v>34969</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1">
         <v>36346</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" s="1">
         <v>37170</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1">
         <v>36739</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G11">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1">
         <v>36927</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="A13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="4">
         <v>36536</v>
       </c>
-      <c r="D13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13">
+      <c r="D13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3">
         <v>12</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
+      <c r="H13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" s="1">
         <v>37515</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -2688,27 +2800,27 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" s="1">
         <v>34566</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G15">
         <v>14</v>
@@ -2717,27 +2829,27 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1">
         <v>34180</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16">
         <v>15</v>
@@ -2746,9 +2858,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="1">
+        <v>35706</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G17">
         <v>16</v>
@@ -2757,9 +2884,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" s="1">
+        <v>35076</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18">
         <v>17</v>
@@ -2768,9 +2910,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="1">
+        <v>36984</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G19">
         <v>18</v>
@@ -2779,24 +2936,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C20" s="1">
         <v>35074</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>19</v>
@@ -2805,273 +2962,666 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F21" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="4">
+        <v>35717</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="3">
         <v>20</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" s="1">
+        <v>37590</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
       <c r="G22">
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="1">
+        <v>35519</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
       <c r="G23">
         <v>22</v>
       </c>
       <c r="H23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="1">
+        <v>37959</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
       <c r="G24">
         <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="1">
+        <v>37031</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
       <c r="G25">
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="1">
+        <v>35791</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" t="s">
+        <v>100</v>
+      </c>
       <c r="G26">
         <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="1">
+        <v>37172</v>
+      </c>
+      <c r="D27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>100</v>
+      </c>
       <c r="G27">
         <v>26</v>
       </c>
       <c r="H27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="1">
+        <v>36377</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
       <c r="G28">
         <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="1">
+        <v>36889</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" t="s">
+        <v>168</v>
+      </c>
       <c r="G29">
         <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="1">
+        <v>36406</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
       <c r="G30">
         <v>29</v>
       </c>
       <c r="H30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4">
         <v>36216</v>
       </c>
-      <c r="F31" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31">
+      <c r="D31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="3">
         <v>30</v>
       </c>
-      <c r="H31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="1">
+        <v>36792</v>
+      </c>
+      <c r="D32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
       <c r="G32">
         <v>31</v>
       </c>
       <c r="H32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="1">
+        <v>36439</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" t="s">
+        <v>100</v>
+      </c>
       <c r="G33">
         <v>32</v>
       </c>
       <c r="H33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
       <c r="G34">
         <v>33</v>
       </c>
       <c r="H34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" t="s">
+        <v>101</v>
+      </c>
       <c r="G35">
         <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G36">
         <v>35</v>
       </c>
       <c r="H36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1">
+        <v>35573</v>
+      </c>
+      <c r="D37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>100</v>
+      </c>
       <c r="G37">
         <v>36</v>
       </c>
       <c r="H37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G38">
         <v>37</v>
       </c>
       <c r="H38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58">
+      <c r="H57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="H58" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G60">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <v>61</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <v>62</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <v>63</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <v>64</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <v>65</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <v>66</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H67" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H68" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="H69" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more contestants' info to Produce 48
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB9FFCC-9A4C-4864-B98F-D39287170652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BDA44E-9D82-4BE6-89DD-AF5215E77AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="243">
   <si>
     <t>Round_Eliminated</t>
   </si>
@@ -570,16 +570,202 @@
     <t>小嶋真子</t>
   </si>
   <si>
-    <t>Matsui Jurina left the show while still in the top 58 ranking.</t>
-  </si>
-  <si>
     <t>Originally from Thailand.</t>
   </si>
   <si>
     <t>Originally from Singapore.</t>
   </si>
   <si>
-    <t>The only contestant from China.</t>
+    <t>Chiba Erii</t>
+  </si>
+  <si>
+    <t>Kojima Mako</t>
+  </si>
+  <si>
+    <t>中西智代梨</t>
+  </si>
+  <si>
+    <t>Nakanishi Chiyori</t>
+  </si>
+  <si>
+    <t>武藤十夢</t>
+  </si>
+  <si>
+    <t>Mutou Tomu</t>
+  </si>
+  <si>
+    <t>Satou Minami</t>
+  </si>
+  <si>
+    <t>佐藤美波</t>
+  </si>
+  <si>
+    <t>岩立沙穗</t>
+  </si>
+  <si>
+    <t>Iwatate Saho</t>
+  </si>
+  <si>
+    <t>尹海率</t>
+  </si>
+  <si>
+    <t>Yoon Hae Sol</t>
+  </si>
+  <si>
+    <t>金素嬉</t>
+  </si>
+  <si>
+    <t>Kim So Hee</t>
+  </si>
+  <si>
+    <t>金慜㥠</t>
+  </si>
+  <si>
+    <t>Kim Min Seo</t>
+  </si>
+  <si>
+    <t>金賢娥</t>
+  </si>
+  <si>
+    <t>Kim Hyun Ah</t>
+  </si>
+  <si>
+    <t>金秀潤</t>
+  </si>
+  <si>
+    <t>Kim Su Yun</t>
+  </si>
+  <si>
+    <t>Lee Ha Eun</t>
+  </si>
+  <si>
+    <t>李河恩</t>
+  </si>
+  <si>
+    <t>金草妍</t>
+  </si>
+  <si>
+    <t>李宥姃</t>
+  </si>
+  <si>
+    <t>One of the two contestants from China.</t>
+  </si>
+  <si>
+    <t>山田野繪</t>
+  </si>
+  <si>
+    <t>Yamada Noe</t>
+  </si>
+  <si>
+    <t>淺井七海</t>
+  </si>
+  <si>
+    <t>Asai Nanami</t>
+  </si>
+  <si>
+    <t>村川緋杏</t>
+  </si>
+  <si>
+    <t>Murakawa Bibian</t>
+  </si>
+  <si>
+    <t>荒卷美咲</t>
+  </si>
+  <si>
+    <t>Aramaki Misaki</t>
+  </si>
+  <si>
+    <t>本村碧唯</t>
+  </si>
+  <si>
+    <t>Motomura Aoi</t>
+  </si>
+  <si>
+    <t>中野郁海</t>
+  </si>
+  <si>
+    <t>Nakano Ikumi</t>
+  </si>
+  <si>
+    <t>Kim Cho Yeon</t>
+  </si>
+  <si>
+    <t>Lee Yu Jeong</t>
+  </si>
+  <si>
+    <t>王珂</t>
+  </si>
+  <si>
+    <t>Wang Ke</t>
+  </si>
+  <si>
+    <t>曹佳賢</t>
+  </si>
+  <si>
+    <t>朴珉志</t>
+  </si>
+  <si>
+    <t>柳旻瑛</t>
+  </si>
+  <si>
+    <t>朴書英</t>
+  </si>
+  <si>
+    <t>黃召硯</t>
+  </si>
+  <si>
+    <t>申帥賢</t>
+  </si>
+  <si>
+    <t>姜多珉</t>
+  </si>
+  <si>
+    <t>尹恩彬</t>
+  </si>
+  <si>
+    <t>崔璉洙</t>
+  </si>
+  <si>
+    <t>月足天音</t>
+  </si>
+  <si>
+    <t>田中美久</t>
+  </si>
+  <si>
+    <t>梅山戀和</t>
+  </si>
+  <si>
+    <t>植村梓</t>
+  </si>
+  <si>
+    <t>松井珠理奈</t>
+  </si>
+  <si>
+    <t>Matsui Jurina</t>
+  </si>
+  <si>
+    <t>Tsukiashi Amane</t>
+  </si>
+  <si>
+    <t>Tanaka Miku</t>
+  </si>
+  <si>
+    <t>Umeyama Kokona</t>
+  </si>
+  <si>
+    <t>Uemura Azusa</t>
+  </si>
+  <si>
+    <t>Left the show after two episodes.</t>
+  </si>
+  <si>
+    <t>Left the show after four episodes, right before the R1 elimination phase.</t>
+  </si>
+  <si>
+    <t>Left the show after seven episodes, right before the R2 elimination phase.</t>
+  </si>
+  <si>
+    <t>Someone else left the show while still in the top 58 ranking.</t>
   </si>
 </sst>
 </file>
@@ -649,13 +835,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,9 +1197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K8" sqref="K8"/>
+      <selection pane="topRight" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1099,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1134,7 +1319,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -2413,11 +2598,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I30" sqref="I30"/>
+      <selection pane="topRight" activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2429,7 +2614,7 @@
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="16.36328125" customWidth="1"/>
-    <col min="9" max="9" width="58.36328125" customWidth="1"/>
+    <col min="9" max="9" width="60.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -2990,19 +3175,19 @@
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>159</v>
       </c>
       <c r="C22" s="1">
         <v>37590</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" t="s">
         <v>105</v>
       </c>
       <c r="F22" t="s">
@@ -3197,7 +3382,7 @@
         <v>6</v>
       </c>
       <c r="I29" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3309,6 +3494,18 @@
       <c r="A34" t="s">
         <v>175</v>
       </c>
+      <c r="B34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" s="1">
+        <v>37921</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
       <c r="F34" t="s">
         <v>101</v>
       </c>
@@ -3323,6 +3520,18 @@
       <c r="A35" t="s">
         <v>176</v>
       </c>
+      <c r="B35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C35" s="1">
+        <v>35580</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>104</v>
+      </c>
       <c r="F35" t="s">
         <v>101</v>
       </c>
@@ -3334,6 +3543,24 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="1">
+        <v>35791</v>
+      </c>
+      <c r="D36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
       <c r="G36">
         <v>35</v>
       </c>
@@ -3368,6 +3595,24 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="1">
+        <v>34831</v>
+      </c>
+      <c r="D38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" t="s">
+        <v>101</v>
+      </c>
       <c r="G38">
         <v>37</v>
       </c>
@@ -3376,6 +3621,24 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="1">
+        <v>34663</v>
+      </c>
+      <c r="D39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
       <c r="G39">
         <v>38</v>
       </c>
@@ -3384,6 +3647,24 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>186</v>
+      </c>
+      <c r="B40" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="1">
+        <v>37836</v>
+      </c>
+      <c r="D40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
+      </c>
       <c r="G40">
         <v>39</v>
       </c>
@@ -3392,6 +3673,24 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" s="1">
+        <v>34611</v>
+      </c>
+      <c r="D41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>101</v>
+      </c>
       <c r="G41">
         <v>40</v>
       </c>
@@ -3400,6 +3699,24 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" s="1">
+        <v>36440</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
       <c r="G42">
         <v>41</v>
       </c>
@@ -3408,6 +3725,24 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="1">
+        <v>36666</v>
+      </c>
+      <c r="D43" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>101</v>
+      </c>
       <c r="G43">
         <v>42</v>
       </c>
@@ -3416,6 +3751,24 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" t="s">
+        <v>192</v>
+      </c>
+      <c r="C44" s="1">
+        <v>37847</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>100</v>
+      </c>
       <c r="G44">
         <v>43</v>
       </c>
@@ -3424,6 +3777,24 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="1">
+        <v>37465</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" t="s">
+        <v>100</v>
+      </c>
       <c r="G45">
         <v>44</v>
       </c>
@@ -3432,6 +3803,24 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="1">
+        <v>36497</v>
+      </c>
+      <c r="D46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" t="s">
+        <v>101</v>
+      </c>
       <c r="G46">
         <v>45</v>
       </c>
@@ -3440,6 +3829,24 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" s="1">
+        <v>34712</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" t="s">
+        <v>100</v>
+      </c>
       <c r="G47">
         <v>46</v>
       </c>
@@ -3448,6 +3855,24 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" t="s">
+        <v>198</v>
+      </c>
+      <c r="C48" s="1">
+        <v>36967</v>
+      </c>
+      <c r="D48" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
       <c r="G48">
         <v>47</v>
       </c>
@@ -3456,6 +3881,24 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="1">
+        <v>38290</v>
+      </c>
+      <c r="D49" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
       <c r="G49">
         <v>48</v>
       </c>
@@ -3464,6 +3907,24 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>210</v>
+      </c>
+      <c r="B50" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="1">
+        <v>36919</v>
+      </c>
+      <c r="D50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" t="s">
+        <v>106</v>
+      </c>
+      <c r="F50" t="s">
+        <v>101</v>
+      </c>
       <c r="G50">
         <v>49</v>
       </c>
@@ -3472,6 +3933,24 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" t="s">
+        <v>216</v>
+      </c>
+      <c r="C51" s="1">
+        <v>37104</v>
+      </c>
+      <c r="D51" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" t="s">
+        <v>100</v>
+      </c>
       <c r="G51">
         <v>50</v>
       </c>
@@ -3480,6 +3959,24 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" t="s">
+        <v>217</v>
+      </c>
+      <c r="C52" s="1">
+        <v>38152</v>
+      </c>
+      <c r="D52" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" t="s">
+        <v>124</v>
+      </c>
+      <c r="F52" t="s">
+        <v>100</v>
+      </c>
       <c r="G52">
         <v>51</v>
       </c>
@@ -3488,6 +3985,24 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C53" s="1">
+        <v>35581</v>
+      </c>
+      <c r="D53" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" t="s">
+        <v>104</v>
+      </c>
+      <c r="F53" t="s">
+        <v>101</v>
+      </c>
       <c r="G53">
         <v>52</v>
       </c>
@@ -3496,6 +4011,12 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" t="s">
+        <v>100</v>
+      </c>
       <c r="G54">
         <v>53</v>
       </c>
@@ -3504,6 +4025,12 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>222</v>
+      </c>
+      <c r="F55" t="s">
+        <v>100</v>
+      </c>
       <c r="G55">
         <v>54</v>
       </c>
@@ -3512,6 +4039,12 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>223</v>
+      </c>
+      <c r="F56" t="s">
+        <v>100</v>
+      </c>
       <c r="G56">
         <v>55</v>
       </c>
@@ -3520,20 +4053,45 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B57" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="1">
+        <v>36835</v>
+      </c>
+      <c r="D57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" t="s">
+        <v>131</v>
+      </c>
+      <c r="F57" t="s">
+        <v>168</v>
+      </c>
       <c r="G57">
         <v>56</v>
       </c>
       <c r="H57" t="s">
         <v>95</v>
       </c>
+      <c r="I57" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="3"/>
+      <c r="A58" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G58" s="3">
         <v>57</v>
       </c>
@@ -3543,37 +4101,73 @@
       <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" t="s">
+        <v>215</v>
+      </c>
+      <c r="C59" s="1">
+        <v>36758</v>
+      </c>
+      <c r="D59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" t="s">
+        <v>101</v>
+      </c>
       <c r="G59">
         <v>59</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" t="s">
         <v>86</v>
       </c>
       <c r="I59" t="s">
-        <v>177</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>224</v>
+      </c>
+      <c r="F60" t="s">
+        <v>100</v>
+      </c>
       <c r="G60">
         <v>60</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>225</v>
+      </c>
+      <c r="F61" t="s">
+        <v>100</v>
+      </c>
       <c r="G61">
         <v>61</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>226</v>
+      </c>
+      <c r="F62" t="s">
+        <v>100</v>
+      </c>
       <c r="G62">
         <v>62</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3581,7 +4175,7 @@
       <c r="G63">
         <v>63</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3589,39 +4183,401 @@
       <c r="G64">
         <v>64</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>227</v>
+      </c>
+      <c r="F65" t="s">
+        <v>100</v>
+      </c>
       <c r="G65">
         <v>65</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>228</v>
+      </c>
+      <c r="F66" t="s">
+        <v>100</v>
+      </c>
       <c r="G66">
         <v>66</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="H67" s="5" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <v>67</v>
+      </c>
+      <c r="H67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="H68" s="5" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G68">
+        <v>68</v>
+      </c>
+      <c r="H68" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="H69" s="5" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G69">
+        <v>69</v>
+      </c>
+      <c r="H69" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>70</v>
+      </c>
+      <c r="H70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <v>71</v>
+      </c>
+      <c r="H71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>72</v>
+      </c>
+      <c r="H72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G73">
+        <v>73</v>
+      </c>
+      <c r="H73" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G74">
+        <v>74</v>
+      </c>
+      <c r="H74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G75">
+        <v>75</v>
+      </c>
+      <c r="H75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G76">
+        <v>76</v>
+      </c>
+      <c r="H76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G77">
+        <v>77</v>
+      </c>
+      <c r="H77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G78">
+        <v>78</v>
+      </c>
+      <c r="H78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G79">
+        <v>79</v>
+      </c>
+      <c r="H79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G80">
+        <v>80</v>
+      </c>
+      <c r="H80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G81">
+        <v>81</v>
+      </c>
+      <c r="H81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G82">
+        <v>82</v>
+      </c>
+      <c r="H82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G83">
+        <v>83</v>
+      </c>
+      <c r="H83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G84">
+        <v>84</v>
+      </c>
+      <c r="H84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G85">
+        <v>85</v>
+      </c>
+      <c r="H85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G86">
+        <v>86</v>
+      </c>
+      <c r="H86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G87">
+        <v>87</v>
+      </c>
+      <c r="H87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G88">
+        <v>88</v>
+      </c>
+      <c r="H88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G89">
+        <v>89</v>
+      </c>
+      <c r="H89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F90" t="s">
+        <v>100</v>
+      </c>
+      <c r="G90">
+        <v>90</v>
+      </c>
+      <c r="H90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G91">
+        <v>91</v>
+      </c>
+      <c r="H91" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G92" s="3">
+        <v>92</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I92" s="3"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>229</v>
+      </c>
+      <c r="B93" t="s">
+        <v>235</v>
+      </c>
+      <c r="C93" s="1">
+        <v>36459</v>
+      </c>
+      <c r="D93" t="s">
+        <v>106</v>
+      </c>
+      <c r="E93" t="s">
+        <v>106</v>
+      </c>
+      <c r="F93" t="s">
+        <v>101</v>
+      </c>
+      <c r="G93">
+        <v>100</v>
+      </c>
+      <c r="H93" t="s">
+        <v>52</v>
+      </c>
+      <c r="I93" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>230</v>
+      </c>
+      <c r="B94" t="s">
+        <v>236</v>
+      </c>
+      <c r="C94" s="1">
+        <v>37146</v>
+      </c>
+      <c r="D94" t="s">
+        <v>106</v>
+      </c>
+      <c r="E94" t="s">
+        <v>124</v>
+      </c>
+      <c r="F94" t="s">
+        <v>101</v>
+      </c>
+      <c r="G94">
+        <v>100</v>
+      </c>
+      <c r="H94" t="s">
+        <v>52</v>
+      </c>
+      <c r="I94" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>231</v>
+      </c>
+      <c r="B95" t="s">
+        <v>237</v>
+      </c>
+      <c r="C95" s="1">
+        <v>37840</v>
+      </c>
+      <c r="D95" t="s">
+        <v>106</v>
+      </c>
+      <c r="E95" t="s">
+        <v>52</v>
+      </c>
+      <c r="F95" t="s">
+        <v>101</v>
+      </c>
+      <c r="G95">
+        <v>100</v>
+      </c>
+      <c r="H95" t="s">
+        <v>52</v>
+      </c>
+      <c r="I95" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>232</v>
+      </c>
+      <c r="B96" t="s">
+        <v>238</v>
+      </c>
+      <c r="C96" s="1">
+        <v>36195</v>
+      </c>
+      <c r="D96" t="s">
+        <v>106</v>
+      </c>
+      <c r="E96" t="s">
+        <v>52</v>
+      </c>
+      <c r="F96" t="s">
+        <v>101</v>
+      </c>
+      <c r="G96">
+        <v>100</v>
+      </c>
+      <c r="H96" t="s">
+        <v>52</v>
+      </c>
+      <c r="I96" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>233</v>
+      </c>
+      <c r="B97" t="s">
+        <v>234</v>
+      </c>
+      <c r="C97" s="1">
+        <v>35497</v>
+      </c>
+      <c r="D97" t="s">
+        <v>104</v>
+      </c>
+      <c r="E97" t="s">
+        <v>104</v>
+      </c>
+      <c r="F97" t="s">
+        <v>101</v>
+      </c>
+      <c r="G97">
+        <v>100</v>
+      </c>
+      <c r="H97" t="s">
+        <v>52</v>
+      </c>
+      <c r="I97" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed the Produce 48 data entry
</commit_message>
<xml_diff>
--- a/UNFINISHED_Idol_School_Dataset.xlsx
+++ b/UNFINISHED_Idol_School_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star1327p\Google Drive\Personal_data\K-Pop-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BDA44E-9D82-4BE6-89DD-AF5215E77AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD820035-B091-42F1-8690-57D837780082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2081691C-6DB5-4FA7-8FC8-9AC7B474A903}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="311">
   <si>
     <t>Round_Eliminated</t>
   </si>
@@ -766,13 +766,217 @@
   </si>
   <si>
     <t>Someone else left the show while still in the top 58 ranking.</t>
+  </si>
+  <si>
+    <t>Park Min Ji</t>
+  </si>
+  <si>
+    <t>Yu Min Young</t>
+  </si>
+  <si>
+    <t>Park Seo Young</t>
+  </si>
+  <si>
+    <t>Cho Ka Hyeon</t>
+  </si>
+  <si>
+    <t>Hwang So Yeon</t>
+  </si>
+  <si>
+    <t>Shin Su Hyun</t>
+  </si>
+  <si>
+    <t>Kang Da Min</t>
+  </si>
+  <si>
+    <t>朴贊珠</t>
+  </si>
+  <si>
+    <t>朴眞熙</t>
+  </si>
+  <si>
+    <t>金多娟</t>
+  </si>
+  <si>
+    <t>趙雅榮</t>
+  </si>
+  <si>
+    <t>李承泫</t>
+  </si>
+  <si>
+    <t>金多蕙</t>
+  </si>
+  <si>
+    <t>洪藝智</t>
+  </si>
+  <si>
+    <t>李彩正</t>
+  </si>
+  <si>
+    <t>朴志殷</t>
+  </si>
+  <si>
+    <t>元書妍</t>
+  </si>
+  <si>
+    <t>Won Seo Yeon</t>
+  </si>
+  <si>
+    <t>茂木忍</t>
+  </si>
+  <si>
+    <t>Mogi Shinobu</t>
+  </si>
+  <si>
+    <t>小田绘里奈</t>
+  </si>
+  <si>
+    <t>Oda Erina</t>
+  </si>
+  <si>
+    <t>松岡菜摘</t>
+  </si>
+  <si>
+    <t>Matsuoka Natsumi</t>
+  </si>
+  <si>
+    <t>長谷川玲奈</t>
+  </si>
+  <si>
+    <t>Hasegawa Rena</t>
+  </si>
+  <si>
+    <t>加藤夕夏</t>
+  </si>
+  <si>
+    <t>Katou Yuuka</t>
+  </si>
+  <si>
+    <t>今田美奈</t>
+  </si>
+  <si>
+    <t>Imada Mina</t>
+  </si>
+  <si>
+    <t>永野芹佳</t>
+  </si>
+  <si>
+    <t>Nagano Serika</t>
+  </si>
+  <si>
+    <t>市川愛美</t>
+  </si>
+  <si>
+    <t>Ichikawa Manami</t>
+  </si>
+  <si>
+    <t>篠崎彩奈</t>
+  </si>
+  <si>
+    <t>Shinozaki Ayana</t>
+  </si>
+  <si>
+    <t>Yoon Eun Bin</t>
+  </si>
+  <si>
+    <t>Choi Yein Soo</t>
+  </si>
+  <si>
+    <t>Park Chan Ju</t>
+  </si>
+  <si>
+    <t>Park Jinny</t>
+  </si>
+  <si>
+    <t>Kim Da Yeon</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>The only contestant from the USA.</t>
+  </si>
+  <si>
+    <t>克利絲汀</t>
+  </si>
+  <si>
+    <t>Alex Christine</t>
+  </si>
+  <si>
+    <t>趙英燕</t>
+  </si>
+  <si>
+    <t>安藝媛</t>
+  </si>
+  <si>
+    <t>金有彬</t>
+  </si>
+  <si>
+    <t>趙思朗</t>
+  </si>
+  <si>
+    <t>崔韶恩</t>
+  </si>
+  <si>
+    <t>Choi So Eun</t>
+  </si>
+  <si>
+    <t>Kim Yu Bin</t>
+  </si>
+  <si>
+    <t>Cho Sa Rang</t>
+  </si>
+  <si>
+    <t>Cho Yeong In</t>
+  </si>
+  <si>
+    <t>Ahn Ye Won</t>
+  </si>
+  <si>
+    <t>栗原紗英</t>
+  </si>
+  <si>
+    <t>淺井裕華</t>
+  </si>
+  <si>
+    <t>內木志</t>
+  </si>
+  <si>
+    <t>Naiki Kokoro</t>
+  </si>
+  <si>
+    <t>Asai Yuuka</t>
+  </si>
+  <si>
+    <t>Kurihara Sae</t>
+  </si>
+  <si>
+    <t>Cho Ah Yeong</t>
+  </si>
+  <si>
+    <t>Lee Seung Hyeon</t>
+  </si>
+  <si>
+    <t>Kim Da Hye</t>
+  </si>
+  <si>
+    <t>Inaccurate birth date. Wikipedia only states that she was born in 2002.</t>
+  </si>
+  <si>
+    <t>Hong Ye Ji</t>
+  </si>
+  <si>
+    <t>Lee Chae Jeong</t>
+  </si>
+  <si>
+    <t>Park Ji Eun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,6 +994,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202122"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,11 +1025,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,7 +1036,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -835,17 +1044,234 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -873,6 +1299,24 @@
     <tableColumn id="9" xr3:uid="{6F48FB8E-8E0D-43BE-A400-3699F2EB1A3A}" name="Final_Rank"/>
     <tableColumn id="10" xr3:uid="{5FDF561D-01D0-4E56-9E88-A9B1D1C3426E}" name="Round_Eliminated"/>
     <tableColumn id="11" xr3:uid="{DC5B0B4A-57F6-42E4-822B-CF800F93543A}" name="Special_Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B25C930A-A6E2-4D7E-9B48-561117C0A8D6}" name="Table2" displayName="Table2" ref="A1:I97" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="11" tableBorderDxfId="12">
+  <autoFilter ref="A1:I97" xr:uid="{B25C930A-A6E2-4D7E-9B48-561117C0A8D6}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{11A41400-9259-4B24-95B2-E3D825109CB4}" name="Name_Chn" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{41704FC7-D228-465B-97B6-F0E47A90B435}" name="Name_Eng" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{EF35BD0A-BFEF-4747-B519-5D818148F536}" name="DOB" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{B99673CC-EF0E-4A40-B15F-DED57CA58A0C}" name="First_Eval" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DB04067B-994B-40D7-858F-C025AE3715C6}" name="Second_Eval" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{133F2ECA-D474-4902-9EC3-5AF62BECAA96}" name="Country" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E91564D7-BFD2-4A0E-867C-7B63FE6AB4D6}" name="Final_Rank" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{4A1B20C5-EA1C-4872-8A83-130A42BA3905}" name="Round_Eliminated" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{C0D95A1C-583E-4027-AEC7-FE2A33DCA342}" name="Special_Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1197,9 +1641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37563BE9-81D1-4F6A-8412-65F577236D71}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I45" sqref="I45"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2600,9 +3044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216AB9D-80AB-4525-8D67-6B7E9AB8E00E}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I65" sqref="I65"/>
+      <selection pane="topRight" activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2610,1978 +3054,2665 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="15.90625" customWidth="1"/>
     <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
     <col min="9" max="9" width="60.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>38230</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>35873</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>37186</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>36432</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>37865</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>37060</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>34969</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2">
         <v>7</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>36346</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="2">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>37170</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>36739</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="2">
         <v>10</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>36927</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="2">
         <v>11</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>36536</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="4">
         <v>12</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>37515</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="2">
         <v>13</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>34566</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>34180</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>15</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>35706</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>16</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>35076</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>17</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <v>36984</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>18</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>35074</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20">
+      <c r="F20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="2">
         <v>19</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>35717</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="4">
         <v>20</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <v>37590</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F22" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2">
         <v>21</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>35519</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>22</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="3">
         <v>37959</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24">
+      <c r="F24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" s="2">
         <v>23</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <v>37031</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>24</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <v>35791</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F26" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="2">
         <v>25</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="3">
         <v>37172</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F27" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27">
+      <c r="F27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="2">
         <v>26</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3">
         <v>36377</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28">
+      <c r="F28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="2">
         <v>27</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="3">
         <v>36889</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>28</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="3">
         <v>36406</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30">
+      <c r="F30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="2">
         <v>29</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>36216</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="4">
         <v>30</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="3"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="3">
         <v>36792</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="2">
         <v>31</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="3">
         <v>36439</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F33" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33">
+      <c r="F33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="2">
         <v>32</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="3">
         <v>37921</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <v>33</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>35580</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2">
         <v>34</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="3">
         <v>35791</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F36" t="s">
-        <v>100</v>
-      </c>
-      <c r="G36">
+      <c r="F36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="2">
         <v>35</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="3">
         <v>35573</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F37" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37">
+      <c r="F37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="2">
         <v>36</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>34831</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <v>37</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="3">
         <v>34663</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <v>38</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="3">
         <v>37836</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <v>39</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="3">
         <v>34611</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>40</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="3">
         <v>36440</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>41</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="3">
         <v>36666</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>42</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="3">
         <v>37847</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F44" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44">
+      <c r="F44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" s="2">
         <v>43</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="3">
         <v>37465</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F45" t="s">
-        <v>100</v>
-      </c>
-      <c r="G45">
+      <c r="F45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="2">
         <v>44</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="3">
         <v>36497</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>45</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="3">
         <v>34712</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F47" t="s">
-        <v>100</v>
-      </c>
-      <c r="G47">
+      <c r="F47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G47" s="2">
         <v>46</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="3">
         <v>36967</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F48" t="s">
-        <v>100</v>
-      </c>
-      <c r="G48">
+      <c r="F48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" s="2">
         <v>47</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="3">
         <v>38290</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49">
+      <c r="F49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="2">
         <v>48</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="3">
         <v>36919</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>49</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="3">
         <v>37104</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F51" t="s">
-        <v>100</v>
-      </c>
-      <c r="G51">
+      <c r="F51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" s="2">
         <v>50</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="3">
         <v>38152</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F52" t="s">
-        <v>100</v>
-      </c>
-      <c r="G52">
+      <c r="F52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" s="2">
         <v>51</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="3">
         <v>35581</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="2">
         <v>52</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F54" t="s">
-        <v>100</v>
-      </c>
-      <c r="G54">
+      <c r="B54" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C54" s="3">
+        <v>36250</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G54" s="2">
         <v>53</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F55" t="s">
-        <v>100</v>
-      </c>
-      <c r="G55">
+      <c r="B55" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C55" s="3">
+        <v>36621</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="2">
         <v>54</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F56" t="s">
-        <v>100</v>
-      </c>
-      <c r="G56">
+      <c r="B56" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" s="3">
+        <v>36229</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="2">
         <v>55</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="3">
         <v>36835</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2">
         <v>56</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G58" s="3">
+      <c r="B58" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C58" s="5">
+        <v>37659</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G58" s="4">
         <v>57</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I58" s="3"/>
+      <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="3">
         <v>36758</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="2">
         <v>59</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F60" t="s">
-        <v>100</v>
-      </c>
-      <c r="G60">
+      <c r="B60" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C60" s="3">
+        <v>36759</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="2">
         <v>60</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F61" t="s">
-        <v>100</v>
-      </c>
-      <c r="G61">
+      <c r="B61" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C61" s="3">
+        <v>35122</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" s="2">
         <v>61</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F62" t="s">
-        <v>100</v>
-      </c>
-      <c r="G62">
+      <c r="B62" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" s="3">
+        <v>38070</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G62" s="2">
         <v>62</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G63">
+      <c r="A63" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="3">
+        <v>35477</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G63" s="2">
         <v>63</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G64">
+      <c r="A64" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C64" s="3">
+        <v>35545</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G64" s="2">
         <v>64</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F65" t="s">
-        <v>100</v>
-      </c>
-      <c r="G65">
+      <c r="B65" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C65" s="3">
+        <v>38128</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G65" s="2">
         <v>65</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F66" t="s">
-        <v>100</v>
-      </c>
-      <c r="G66">
+      <c r="B66" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C66" s="3">
+        <v>36356</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G66" s="2">
         <v>66</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G67">
+      <c r="I66" s="2"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C67" s="3">
+        <v>35285</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G67" s="2">
         <v>67</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G68">
+      <c r="I67" s="2"/>
+    </row>
+    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.4">
+      <c r="A68" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C68" s="3">
+        <v>36492</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G68" s="2">
         <v>68</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G69">
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C69" s="3">
+        <v>35814</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G69" s="2">
         <v>69</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G70">
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C70" s="3">
+        <v>37682</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G70" s="2">
         <v>70</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G71">
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C71" s="3">
+        <v>36965</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G71" s="2">
         <v>71</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G72">
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="3">
+        <v>36808</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G72" s="2">
         <v>72</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G73">
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C73" s="3">
+        <v>36943</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G73" s="2">
         <v>73</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G74">
+      <c r="I73" s="2"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C74" s="3">
+        <v>35643</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G74" s="2">
         <v>74</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G75">
+      <c r="I74" s="2"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C75" s="3">
+        <v>37257</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G75" s="2">
         <v>75</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G76">
+      <c r="I75" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C76" s="3">
+        <v>35494</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G76" s="2">
         <v>76</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G77">
+      <c r="I76" s="2"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C77" s="3">
+        <v>36977</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G77" s="2">
         <v>77</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G78">
+      <c r="I77" s="2"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C78" s="3">
+        <v>37287</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G78" s="2">
         <v>78</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G79">
+      <c r="I78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C79" s="3">
+        <v>36399</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G79" s="2">
         <v>79</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G80">
+      <c r="I79" s="2"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C80" s="3">
+        <v>35677</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G80" s="2">
         <v>80</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G81">
+      <c r="A81" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C81" s="3">
+        <v>36398</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G81" s="2">
         <v>81</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I81" s="2"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G82">
+      <c r="A82" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C82" s="3">
+        <v>35408</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G82" s="2">
         <v>82</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I82" s="2" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G83">
+      <c r="A83" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C83" s="3">
+        <v>35236</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G83" s="2">
         <v>83</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G84">
+      <c r="A84" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C84" s="3">
+        <v>37195</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G84" s="2">
         <v>84</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G85">
+      <c r="A85" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C85" s="3">
+        <v>37935</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G85" s="2">
         <v>85</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G86">
+      <c r="A86" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C86" s="3">
+        <v>36932</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G86" s="2">
         <v>86</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I86" s="2"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G87">
+      <c r="A87" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C87" s="3">
+        <v>35526</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G87" s="2">
         <v>87</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H87" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G88">
+      <c r="A88" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C88" s="3">
+        <v>37679</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G88" s="2">
         <v>88</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H88" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G89">
+      <c r="A89" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C89" s="3">
+        <v>37869</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G89" s="2">
         <v>89</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F90" t="s">
-        <v>100</v>
-      </c>
-      <c r="G90">
+      <c r="A90" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C90" s="3">
+        <v>37153</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G90" s="2">
         <v>90</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G91">
+      <c r="A91" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C91" s="3">
+        <v>35072</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G91" s="2">
         <v>91</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G92" s="3">
+      <c r="A92" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="5">
+        <v>36669</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G92" s="4">
         <v>92</v>
       </c>
-      <c r="H92" s="3" t="s">
+      <c r="H92" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I92" s="3"/>
+      <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="A93" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="3">
         <v>36459</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G93">
-        <v>100</v>
-      </c>
-      <c r="H93" t="s">
+      <c r="G93" s="2">
+        <v>100</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="A94" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="3">
         <v>37146</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G94">
-        <v>100</v>
-      </c>
-      <c r="H94" t="s">
+      <c r="G94" s="2">
+        <v>100</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" s="2" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="A95" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="3">
         <v>37840</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G95">
-        <v>100</v>
-      </c>
-      <c r="H95" t="s">
+      <c r="G95" s="2">
+        <v>100</v>
+      </c>
+      <c r="H95" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I95" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+      <c r="A96" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="3">
         <v>36195</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G96">
-        <v>100</v>
-      </c>
-      <c r="H96" t="s">
+      <c r="G96" s="2">
+        <v>100</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="A97" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="3">
         <v>35497</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G97">
-        <v>100</v>
-      </c>
-      <c r="H97" t="s">
+      <c r="G97" s="2">
+        <v>100</v>
+      </c>
+      <c r="H97" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="2" t="s">
         <v>241</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>